<commit_message>
Second version of dashboards
</commit_message>
<xml_diff>
--- a/Afternoon shift.xlsx
+++ b/Afternoon shift.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -46,70 +46,58 @@
     <t>Rate</t>
   </si>
   <si>
+    <t>Janeth,Falquez</t>
+  </si>
+  <si>
+    <t>Wayne,Frederick</t>
+  </si>
+  <si>
     <t>Daquan,Bryant</t>
   </si>
   <si>
-    <t>Brien,McDonnell</t>
-  </si>
-  <si>
-    <t>Luis,Naula Jara</t>
+    <t>Quinndel,Scott-Wright</t>
+  </si>
+  <si>
+    <t>David,Sosa Jr.</t>
+  </si>
+  <si>
+    <t>Alina,Castillo Alcantara</t>
+  </si>
+  <si>
+    <t>Edison,Rodriguez Gonzalez</t>
+  </si>
+  <si>
+    <t>Yave,Caba Corona</t>
   </si>
   <si>
     <t>Jose,Guaman</t>
   </si>
   <si>
-    <t>Janeth,Falquez</t>
-  </si>
-  <si>
-    <t>Nana,Dompo</t>
-  </si>
-  <si>
-    <t>Wayne,Frederick</t>
+    <t>David,Ojeda Herrera</t>
   </si>
   <si>
     <t>Jose,Correa</t>
   </si>
   <si>
-    <t>David,Ojeda Herrera</t>
-  </si>
-  <si>
-    <t>Michael,Cater</t>
-  </si>
-  <si>
-    <t>Rodolfo,Mendoza</t>
-  </si>
-  <si>
-    <t>Quinndel,Scott-Wright</t>
-  </si>
-  <si>
-    <t>107.00</t>
-  </si>
-  <si>
-    <t>87.00</t>
-  </si>
-  <si>
-    <t>63.00</t>
-  </si>
-  <si>
-    <t>62.00</t>
-  </si>
-  <si>
-    <t>57.50</t>
-  </si>
-  <si>
-    <t>44.00</t>
+    <t>Tony,Soler Tatis</t>
+  </si>
+  <si>
+    <t>109.00</t>
+  </si>
+  <si>
+    <t>96.00</t>
+  </si>
+  <si>
+    <t>91.00</t>
+  </si>
+  <si>
+    <t>83.00</t>
+  </si>
+  <si>
+    <t>70.00</t>
   </si>
   <si>
     <t>41.00</t>
-  </si>
-  <si>
-    <t>32.00</t>
-  </si>
-  <si>
-    <t>30.00</t>
-  </si>
-  <si>
-    <t>27.00</t>
   </si>
   <si>
     <t>24.00</t>
@@ -519,10 +507,10 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -554,7 +542,7 @@
         <v>11</v>
       </c>
       <c r="C3">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -589,7 +577,7 @@
         <v>12</v>
       </c>
       <c r="C4">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -624,10 +612,10 @@
         <v>13</v>
       </c>
       <c r="C5">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -659,10 +647,10 @@
         <v>14</v>
       </c>
       <c r="C6">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D6">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -694,10 +682,10 @@
         <v>15</v>
       </c>
       <c r="C7">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D7">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -729,10 +717,10 @@
         <v>16</v>
       </c>
       <c r="C8">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -764,22 +752,22 @@
         <v>17</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -799,13 +787,13 @@
         <v>18</v>
       </c>
       <c r="C10">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D10">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -823,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -834,31 +822,31 @@
         <v>19</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
         <v>29</v>
-      </c>
-      <c r="E11">
-        <v>25</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -869,13 +857,13 @@
         <v>20</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D12">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -893,7 +881,7 @@
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -904,10 +892,10 @@
         <v>21</v>
       </c>
       <c r="C13">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -928,7 +916,7 @@
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>